<commit_message>
updated fx con excel file
</commit_message>
<xml_diff>
--- a/fMRI/fx/models/all_emotions/contrasts.xlsx
+++ b/fMRI/fx/models/all_emotions/contrasts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11500" yWindow="5940" windowWidth="36180" windowHeight="19600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>A</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Artefact</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,6 +615,41 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>